<commit_message>
Got 70% coverage and correct stacking working now; just packing short SKUs last now
</commit_message>
<xml_diff>
--- a/new_data/Optimized_Bundles.xlsx
+++ b/new_data/Optimized_Bundles.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="1" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SO_Input_Old" sheetId="1" state="visible" r:id="rId1"/>
@@ -367,7 +367,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D117" headerRowCount="1" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:D117"/>
+  <autoFilter ref="A1:D117">
+    <filterColumn colId="0" hiddenButton="0" showButton="1">
+      <filters>
+        <filter val="SO-1013166"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" name="Order ID" dataDxfId="4"/>
     <tableColumn id="2" name="SKU" dataDxfId="3"/>
@@ -739,7 +745,7 @@
   </sheetPr>
   <dimension ref="A1:H117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3951,8 +3957,8 @@
   </sheetPr>
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -3986,7 +3992,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1" s="6">
       <c r="A2" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4001,7 +4007,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1" s="6">
       <c r="A3" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -4016,7 +4022,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="1" s="6">
       <c r="A4" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -4031,7 +4037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="1" s="6">
       <c r="A5" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4046,7 +4052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="1" s="6">
       <c r="A6" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4061,7 +4067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="1" s="6">
       <c r="A7" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4076,7 +4082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="1" s="6">
       <c r="A8" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4091,7 +4097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="1" s="6">
       <c r="A9" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4121,7 +4127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="1" s="6">
       <c r="A11" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -4136,7 +4142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="1" s="6">
       <c r="A12" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4151,7 +4157,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="1" s="6">
       <c r="A13" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4166,7 +4172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="1" s="6">
       <c r="A14" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -4181,7 +4187,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1" s="6">
       <c r="A15" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4196,7 +4202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="1" s="6">
       <c r="A16" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4211,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="1" s="6">
       <c r="A17" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4226,7 +4232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="1" s="6">
       <c r="A18" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4241,7 +4247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="1" s="6">
       <c r="A19" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4256,7 +4262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="1" s="6">
       <c r="A20" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -4271,7 +4277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="1" s="6">
       <c r="A21" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -4286,7 +4292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="1" s="6">
       <c r="A22" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4301,7 +4307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="1" s="6">
       <c r="A23" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4316,7 +4322,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="1" s="6">
       <c r="A24" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4331,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="1" s="6">
       <c r="A25" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -4346,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="1" s="6">
       <c r="A26" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4361,7 +4367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1" s="6">
       <c r="A27" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4376,7 +4382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="1" s="6">
       <c r="A28" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4391,7 +4397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1" s="6">
       <c r="A29" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4406,7 +4412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="1" s="6">
       <c r="A30" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4421,7 +4427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1" s="6">
       <c r="A31" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -4436,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="1" s="6">
       <c r="A32" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4451,7 +4457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="1" s="6">
       <c r="A33" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4466,7 +4472,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="1" s="6">
       <c r="A34" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4481,7 +4487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="1" s="6">
       <c r="A35" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4496,7 +4502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="1" s="6">
       <c r="A36" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -4511,7 +4517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="1" s="6">
       <c r="A37" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4526,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="1" s="6">
       <c r="A38" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4541,7 +4547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="1" s="6">
       <c r="A39" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4556,7 +4562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="1" s="6">
       <c r="A40" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4571,7 +4577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="1" s="6">
       <c r="A41" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4586,7 +4592,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="1" s="6">
       <c r="A42" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4601,7 +4607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="1" s="6">
       <c r="A43" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -4616,7 +4622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="1" s="6">
       <c r="A44" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4631,7 +4637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="1" s="6">
       <c r="A45" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4646,7 +4652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="1" s="6">
       <c r="A46" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4661,7 +4667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="1" s="6">
       <c r="A47" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4676,7 +4682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="1" s="6">
       <c r="A48" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -4706,7 +4712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="1" s="6">
       <c r="A50" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -4721,7 +4727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="1" s="6">
       <c r="A51" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4736,7 +4742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="1" s="6">
       <c r="A52" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4751,7 +4757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="1" s="6">
       <c r="A53" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4766,7 +4772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="1" s="6">
       <c r="A54" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4796,7 +4802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="1" s="6">
       <c r="A56" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -4811,7 +4817,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="1" s="6">
       <c r="A57" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4826,7 +4832,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="1" s="6">
       <c r="A58" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -4856,7 +4862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="1" s="6">
       <c r="A60" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -4871,7 +4877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="1" s="6">
       <c r="A61" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -4886,7 +4892,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="1" s="6">
       <c r="A62" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -4901,7 +4907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="1" s="6">
       <c r="A63" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -4916,7 +4922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="1" s="6">
       <c r="A64" t="inlineStr">
         <is>
           <t>SO-1013129</t>
@@ -4931,7 +4937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="1" s="6">
       <c r="A65" t="inlineStr">
         <is>
           <t>SO-1013131</t>
@@ -4946,7 +4952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="1" s="6">
       <c r="A66" t="inlineStr">
         <is>
           <t>SO-1013133</t>
@@ -4961,7 +4967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="1" s="6">
       <c r="A67" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4976,7 +4982,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="1" s="6">
       <c r="A68" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -4991,7 +4997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="1" s="6">
       <c r="A69" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -5006,7 +5012,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="1" s="6">
       <c r="A70" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5021,7 +5027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="1" s="6">
       <c r="A71" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5036,7 +5042,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="1" s="6">
       <c r="A72" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5051,7 +5057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="1" s="6">
       <c r="A73" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5066,7 +5072,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="1" s="6">
       <c r="A74" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5081,7 +5087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="1" s="6">
       <c r="A75" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5096,7 +5102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="1" s="6">
       <c r="A76" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5111,7 +5117,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="1" s="6">
       <c r="A77" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5126,7 +5132,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="1" s="6">
       <c r="A78" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -5141,7 +5147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="1" s="6">
       <c r="A79" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -5156,7 +5162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="1" s="6">
       <c r="A80" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5171,7 +5177,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="1" s="6">
       <c r="A81" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5186,7 +5192,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="1" s="6">
       <c r="A82" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5201,7 +5207,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="1" s="6">
       <c r="A83" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5216,7 +5222,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="1" s="6">
       <c r="A84" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5231,7 +5237,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="1" s="6">
       <c r="A85" t="inlineStr">
         <is>
           <t>SO-1013129</t>
@@ -5246,7 +5252,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="1" s="6">
       <c r="A86" t="inlineStr">
         <is>
           <t>SO-1013131</t>
@@ -5261,7 +5267,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="1" s="6">
       <c r="A87" t="inlineStr">
         <is>
           <t>SO-1013133</t>
@@ -5276,7 +5282,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="1" s="6">
       <c r="A88" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5291,7 +5297,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="1" s="6">
       <c r="A89" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -5306,7 +5312,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="1" s="6">
       <c r="A90" t="inlineStr">
         <is>
           <t>SO-1013178</t>
@@ -5321,7 +5327,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="1" s="6">
       <c r="A91" t="inlineStr">
         <is>
           <t>SO-1013179</t>
@@ -5336,7 +5342,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="1" s="6">
       <c r="A92" t="inlineStr">
         <is>
           <t>SO-1013190</t>
@@ -5351,7 +5357,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="1" s="6">
       <c r="A93" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5366,7 +5372,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="1" s="6">
       <c r="A94" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -5396,7 +5402,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="1" s="6">
       <c r="A96" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5411,7 +5417,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="1" s="6">
       <c r="A97" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5426,7 +5432,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="1" s="6">
       <c r="A98" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5441,7 +5447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="1" s="6">
       <c r="A99" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5456,7 +5462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="1" s="6">
       <c r="A100" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5471,7 +5477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="1" s="6">
       <c r="A101" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5486,7 +5492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="1" s="6">
       <c r="A102" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5501,7 +5507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="1" s="6">
       <c r="A103" t="inlineStr">
         <is>
           <t>SO-1013122</t>
@@ -5516,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="1" s="6">
       <c r="A104" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5546,7 +5552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="1" s="6">
       <c r="A106" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -5561,7 +5567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" hidden="1" s="6">
       <c r="A107" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5576,7 +5582,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" hidden="1" s="6">
       <c r="A108" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5591,7 +5597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" hidden="1" s="6">
       <c r="A109" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5606,7 +5612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" hidden="1" s="6">
       <c r="A110" t="inlineStr">
         <is>
           <t>SO-1013111</t>
@@ -5621,7 +5627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" hidden="1" s="6">
       <c r="A111" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5651,7 +5657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" hidden="1" s="6">
       <c r="A113" t="inlineStr">
         <is>
           <t>SO-1013210</t>
@@ -5666,7 +5672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" hidden="1" s="6">
       <c r="A114" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5681,7 +5687,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" hidden="1" s="6">
       <c r="A115" t="inlineStr">
         <is>
           <t>SO-1013206</t>
@@ -5711,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" hidden="1" s="6">
       <c r="A117" t="inlineStr">
         <is>
           <t>SO-1013148</t>
@@ -5742,8 +5748,8 @@
   </sheetPr>
   <dimension ref="A1:F267"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A259" sqref="A259"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="K204" sqref="K204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -10837,7 +10843,7 @@
         <v>228.6</v>
       </c>
       <c r="I20" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J20" t="inlineStr"/>
     </row>
@@ -10868,7 +10874,7 @@
         <v>228.6</v>
       </c>
       <c r="I21" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J21" t="inlineStr"/>
     </row>
@@ -10899,7 +10905,7 @@
         <v>228.6</v>
       </c>
       <c r="I22" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J22" t="inlineStr"/>
     </row>
@@ -10930,7 +10936,7 @@
         <v>228.6</v>
       </c>
       <c r="I23" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J23" t="inlineStr"/>
     </row>
@@ -10961,7 +10967,7 @@
         <v>228.6</v>
       </c>
       <c r="I24" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J24" t="inlineStr"/>
     </row>
@@ -10992,7 +10998,7 @@
         <v>228.6</v>
       </c>
       <c r="I25" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J25" t="inlineStr"/>
     </row>
@@ -11011,7 +11017,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E26" t="n">
         <v>100</v>
@@ -11023,7 +11029,7 @@
         <v>228.6</v>
       </c>
       <c r="I26" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J26" t="inlineStr"/>
     </row>
@@ -11059,7 +11065,7 @@
         <v>228.6</v>
       </c>
       <c r="I27" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J27" t="inlineStr"/>
     </row>
@@ -11095,7 +11101,7 @@
         <v>228.6</v>
       </c>
       <c r="I28" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J28" t="inlineStr"/>
     </row>
@@ -11131,7 +11137,7 @@
         <v>228.6</v>
       </c>
       <c r="I29" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J29" t="inlineStr"/>
     </row>
@@ -11167,7 +11173,7 @@
         <v>228.6</v>
       </c>
       <c r="I30" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J30" t="inlineStr"/>
     </row>
@@ -11203,7 +11209,7 @@
         <v>228.6</v>
       </c>
       <c r="I31" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J31" t="inlineStr"/>
     </row>
@@ -11239,7 +11245,7 @@
         <v>228.6</v>
       </c>
       <c r="I32" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J32" t="inlineStr"/>
     </row>
@@ -11254,18 +11260,18 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Pack_62Filler</t>
+          <t>Pack_44Filler</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Pack 62 Filler Material</t>
+          <t>Pack 44 Filler Material</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -11275,40 +11281,45 @@
         <v>228.6</v>
       </c>
       <c r="I33" t="n">
-        <v>445.4717959183673</v>
+        <v>438.3929070294784</v>
       </c>
       <c r="J33" t="inlineStr"/>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>SO-1013206</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>1</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>6VR.289.15WCD</t>
-        </is>
-      </c>
-      <c r="D35" t="n">
-        <v>29</v>
-      </c>
-      <c r="E35" t="n">
-        <v>8</v>
-      </c>
-      <c r="G35" t="n">
-        <v>571.5</v>
-      </c>
-      <c r="H35" t="n">
-        <v>584.2</v>
-      </c>
-      <c r="I35" t="n">
-        <v>1672.137609977324</v>
-      </c>
-      <c r="J35" t="inlineStr"/>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>SO-1013179</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Pack_62Filler</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Pack 62 Filler Material</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>565.1500000000001</v>
+      </c>
+      <c r="H34" t="n">
+        <v>228.6</v>
+      </c>
+      <c r="I34" t="n">
+        <v>438.3929070294784</v>
+      </c>
+      <c r="J34" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -11321,14 +11332,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2SS.145.15WCD</t>
+          <t>6VR.289.15WCD</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E36" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G36" t="n">
         <v>571.5</v>
@@ -11352,14 +11363,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3VP.145.15WCD</t>
+          <t>2SS.145.15WCD</t>
         </is>
       </c>
       <c r="D37" t="n">
         <v>2</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G37" t="n">
         <v>571.5</v>
@@ -11383,14 +11394,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1TJT.145.15WCD</t>
+          <t>3VP.145.15WCD</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G38" t="n">
         <v>571.5</v>
@@ -11414,14 +11425,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>JT23.145.15WCD</t>
+          <t>1TJT.145.15WCD</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E39" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G39" t="n">
         <v>571.5</v>
@@ -11445,14 +11456,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2COR1.145.15WCD</t>
+          <t>JT23.145.15WCD</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G40" t="n">
         <v>571.5</v>
@@ -11476,14 +11487,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>JT23C.145.15WCD</t>
+          <t>2COR1.145.15WCD</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G41" t="n">
         <v>571.5</v>
@@ -11507,19 +11518,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>JT23C.145.15WCD</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>20</v>
       </c>
       <c r="G42" t="n">
         <v>571.5</v>
@@ -11543,7 +11549,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -11554,7 +11560,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -11579,7 +11585,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -11590,7 +11596,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -11615,7 +11621,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -11626,7 +11632,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -11651,7 +11657,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -11662,7 +11668,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -11687,18 +11693,18 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
         <v>1</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -11719,27 +11725,32 @@
         </is>
       </c>
       <c r="B48" t="n">
+        <v>1</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Pack_Pad_19_3680</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
         <v>2</v>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>2COR1.145.15WCD</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>1</v>
-      </c>
       <c r="E48" t="n">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+        </is>
       </c>
       <c r="G48" t="n">
-        <v>558.8</v>
+        <v>571.5</v>
       </c>
       <c r="H48" t="n">
-        <v>196.85</v>
+        <v>584.2</v>
       </c>
       <c r="I48" t="n">
-        <v>199.4845487528345</v>
+        <v>1672.137609977324</v>
       </c>
       <c r="J48" t="inlineStr"/>
     </row>
@@ -11754,14 +11765,14 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>2BA.145.15OBL</t>
+          <t>2COR1.145.15WCD</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G49" t="n">
         <v>558.8</v>
@@ -11785,14 +11796,14 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>JT23C.145.15WCD</t>
+          <t>2BA.145.15OBL</t>
         </is>
       </c>
       <c r="D50" t="n">
         <v>2</v>
       </c>
       <c r="E50" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G50" t="n">
         <v>558.8</v>
@@ -11816,14 +11827,14 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2OFFC.145.15WCD</t>
+          <t>JT23C.145.15WCD</t>
         </is>
       </c>
       <c r="D51" t="n">
         <v>2</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G51" t="n">
         <v>558.8</v>
@@ -11847,14 +11858,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CLIP.N1500</t>
+          <t>2OFFC.145.15WCD</t>
         </is>
       </c>
       <c r="D52" t="n">
         <v>2</v>
       </c>
       <c r="E52" t="n">
-        <v>1500</v>
+        <v>10</v>
       </c>
       <c r="G52" t="n">
         <v>558.8</v>
@@ -11878,14 +11889,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2TB.145.15WCD</t>
+          <t>CLIP.N1500</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E53" t="n">
-        <v>10</v>
+        <v>1500</v>
       </c>
       <c r="G53" t="n">
         <v>558.8</v>
@@ -11909,11 +11920,11 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2FR.145.15WCD</t>
+          <t>2TB.145.15WCD</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E54" t="n">
         <v>10</v>
@@ -11940,14 +11951,14 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2COR2.145.15WCD</t>
+          <t>2FR.145.15WCD</t>
         </is>
       </c>
       <c r="D55" t="n">
         <v>2</v>
       </c>
       <c r="E55" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G55" t="n">
         <v>558.8</v>
@@ -11971,7 +11982,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>1OC.145.15WCD</t>
+          <t>2COR2.145.15WCD</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -12002,19 +12013,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>1OC.145.15WCD</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>1</v>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>4</v>
       </c>
       <c r="G57" t="n">
         <v>558.8</v>
@@ -12038,7 +12044,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -12049,7 +12055,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -12074,7 +12080,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -12085,7 +12091,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -12110,7 +12116,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -12121,7 +12127,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G60" t="n">
@@ -12146,7 +12152,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -12157,7 +12163,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G61" t="n">
@@ -12182,18 +12188,18 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E62" t="n">
         <v>1</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -12207,36 +12213,41 @@
       </c>
       <c r="J62" t="inlineStr"/>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>SO-1013190</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>1</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>6VR.289.15DNW</t>
-        </is>
-      </c>
-      <c r="D64" t="n">
-        <v>7</v>
-      </c>
-      <c r="E64" t="n">
-        <v>8</v>
-      </c>
-      <c r="G64" t="n">
-        <v>577.8500000000001</v>
-      </c>
-      <c r="H64" t="n">
-        <v>203.2</v>
-      </c>
-      <c r="I64" t="n">
-        <v>450.0886757369614</v>
-      </c>
-      <c r="J64" t="inlineStr"/>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SO-1013206</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Pack_Pad_19_3680</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>2</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>558.8</v>
+      </c>
+      <c r="H63" t="n">
+        <v>196.85</v>
+      </c>
+      <c r="I63" t="n">
+        <v>199.4845487528345</v>
+      </c>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -12249,14 +12260,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2TJT.145.15DNW</t>
+          <t>6VR.289.15DNW</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E65" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G65" t="n">
         <v>577.8500000000001</v>
@@ -12265,7 +12276,7 @@
         <v>203.2</v>
       </c>
       <c r="I65" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J65" t="inlineStr"/>
     </row>
@@ -12280,11 +12291,11 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1TJT.145.15DNW</t>
+          <t>2TJT.145.15DNW</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E66" t="n">
         <v>20</v>
@@ -12296,7 +12307,7 @@
         <v>203.2</v>
       </c>
       <c r="I66" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J66" t="inlineStr"/>
     </row>
@@ -12311,14 +12322,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>1SJT.145.15DNW</t>
+          <t>1TJT.145.15DNW</t>
         </is>
       </c>
       <c r="D67" t="n">
         <v>1</v>
       </c>
       <c r="E67" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G67" t="n">
         <v>577.8500000000001</v>
@@ -12327,7 +12338,7 @@
         <v>203.2</v>
       </c>
       <c r="I67" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J67" t="inlineStr"/>
     </row>
@@ -12342,11 +12353,11 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2TB.145.15DNW</t>
+          <t>1SJT.145.15DNW</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E68" t="n">
         <v>10</v>
@@ -12358,7 +12369,7 @@
         <v>203.2</v>
       </c>
       <c r="I68" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J68" t="inlineStr"/>
     </row>
@@ -12373,14 +12384,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>2TB.145.15DNW</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E69" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G69" t="n">
         <v>577.8500000000001</v>
@@ -12389,7 +12400,7 @@
         <v>203.2</v>
       </c>
       <c r="I69" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J69" t="inlineStr"/>
     </row>
@@ -12404,19 +12415,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E70" t="n">
-        <v>1</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G70" t="n">
         <v>577.8500000000001</v>
@@ -12425,7 +12431,7 @@
         <v>203.2</v>
       </c>
       <c r="I70" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J70" t="inlineStr"/>
     </row>
@@ -12440,7 +12446,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -12451,7 +12457,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G71" t="n">
@@ -12461,7 +12467,7 @@
         <v>203.2</v>
       </c>
       <c r="I71" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J71" t="inlineStr"/>
     </row>
@@ -12476,7 +12482,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -12487,7 +12493,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G72" t="n">
@@ -12497,7 +12503,7 @@
         <v>203.2</v>
       </c>
       <c r="I72" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J72" t="inlineStr"/>
     </row>
@@ -12512,7 +12518,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -12523,7 +12529,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G73" t="n">
@@ -12533,7 +12539,7 @@
         <v>203.2</v>
       </c>
       <c r="I73" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J73" t="inlineStr"/>
     </row>
@@ -12548,7 +12554,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -12559,7 +12565,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G74" t="n">
@@ -12569,7 +12575,7 @@
         <v>203.2</v>
       </c>
       <c r="I74" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J74" t="inlineStr"/>
     </row>
@@ -12584,18 +12590,18 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="n">
         <v>1</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G75" t="n">
@@ -12605,7 +12611,7 @@
         <v>203.2</v>
       </c>
       <c r="I75" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J75" t="inlineStr"/>
     </row>
@@ -12620,7 +12626,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Pack_44Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -12631,7 +12637,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Pack 44 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G76" t="n">
@@ -12641,40 +12647,45 @@
         <v>203.2</v>
       </c>
       <c r="I76" t="n">
-        <v>450.0886757369614</v>
+        <v>443.1045487528344</v>
       </c>
       <c r="J76" t="inlineStr"/>
     </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>SO-1013166</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>1</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>6PSP.289.15LCY</t>
-        </is>
-      </c>
-      <c r="D78" t="n">
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SO-1013190</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Pack_44Filler</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
         <v>2</v>
       </c>
-      <c r="E78" t="n">
-        <v>8</v>
-      </c>
-      <c r="G78" t="n">
-        <v>533.4</v>
-      </c>
-      <c r="H78" t="n">
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Pack 44 Filler Material</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>577.8500000000001</v>
+      </c>
+      <c r="H77" t="n">
         <v>203.2</v>
       </c>
-      <c r="I78" t="n">
-        <v>269.9566802721088</v>
-      </c>
-      <c r="J78" t="inlineStr"/>
+      <c r="I77" t="n">
+        <v>443.1045487528344</v>
+      </c>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -12687,23 +12698,23 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2X8LLHD.289.15LCY</t>
+          <t>6PSP.289.15LCY</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E79" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G79" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H79" t="n">
         <v>203.2</v>
       </c>
       <c r="I79" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J79" t="inlineStr"/>
     </row>
@@ -12718,23 +12729,23 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>1TJT.145.15LCY</t>
+          <t>2X8LLHD.289.15LCY</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E80" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G80" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H80" t="n">
         <v>203.2</v>
       </c>
       <c r="I80" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J80" t="inlineStr"/>
     </row>
@@ -12749,23 +12760,23 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>JT23.145.15LCY</t>
+          <t>1TJT.145.15LCY</t>
         </is>
       </c>
       <c r="D81" t="n">
         <v>1</v>
       </c>
       <c r="E81" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G81" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H81" t="n">
         <v>203.2</v>
       </c>
       <c r="I81" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J81" t="inlineStr"/>
     </row>
@@ -12780,23 +12791,23 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>JT23C.145.15LCY</t>
+          <t>JT23.145.15LCY</t>
         </is>
       </c>
       <c r="D82" t="n">
         <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G82" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H82" t="n">
         <v>203.2</v>
       </c>
       <c r="I82" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J82" t="inlineStr"/>
     </row>
@@ -12811,23 +12822,23 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2TB.145.15LCY</t>
+          <t>JT23C.145.15LCY</t>
         </is>
       </c>
       <c r="D83" t="n">
         <v>1</v>
       </c>
       <c r="E83" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G83" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H83" t="n">
         <v>203.2</v>
       </c>
       <c r="I83" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J83" t="inlineStr"/>
     </row>
@@ -12842,7 +12853,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>TGBJKIT</t>
+          <t>2TB.145.15LCY</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -12852,13 +12863,13 @@
         <v>10</v>
       </c>
       <c r="G84" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H84" t="n">
         <v>203.2</v>
       </c>
       <c r="I84" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J84" t="inlineStr"/>
     </row>
@@ -12873,23 +12884,23 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>TGBJKIT</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E85" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G85" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H85" t="n">
         <v>203.2</v>
       </c>
       <c r="I85" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J85" t="inlineStr"/>
     </row>
@@ -12904,28 +12915,23 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E86" t="n">
-        <v>1</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G86" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H86" t="n">
         <v>203.2</v>
       </c>
       <c r="I86" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J86" t="inlineStr"/>
     </row>
@@ -12940,7 +12946,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -12951,17 +12957,17 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H87" t="n">
         <v>203.2</v>
       </c>
       <c r="I87" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J87" t="inlineStr"/>
     </row>
@@ -12976,7 +12982,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D88" t="n">
@@ -12987,17 +12993,17 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H88" t="n">
         <v>203.2</v>
       </c>
       <c r="I88" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J88" t="inlineStr"/>
     </row>
@@ -13012,7 +13018,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -13023,17 +13029,17 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H89" t="n">
         <v>203.2</v>
       </c>
       <c r="I89" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J89" t="inlineStr"/>
     </row>
@@ -13048,7 +13054,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D90" t="n">
@@ -13059,17 +13065,17 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H90" t="n">
         <v>203.2</v>
       </c>
       <c r="I90" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J90" t="inlineStr"/>
     </row>
@@ -13084,28 +13090,28 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
         <v>1</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H91" t="n">
         <v>203.2</v>
       </c>
       <c r="I91" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J91" t="inlineStr"/>
     </row>
@@ -13120,61 +13126,66 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Pack_44Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E92" t="n">
         <v>1</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Pack 44 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>533.4</v>
+        <v>508</v>
       </c>
       <c r="H92" t="n">
         <v>203.2</v>
       </c>
       <c r="I92" t="n">
-        <v>269.9566802721088</v>
+        <v>268.6868390022676</v>
       </c>
       <c r="J92" t="inlineStr"/>
     </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>SO-1013210</t>
-        </is>
-      </c>
-      <c r="B94" t="n">
-        <v>1</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>6VR.145.15LNW</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>3</v>
-      </c>
-      <c r="E94" t="n">
-        <v>8</v>
-      </c>
-      <c r="G94" t="n">
-        <v>406.4</v>
-      </c>
-      <c r="H94" t="n">
-        <v>177.8</v>
-      </c>
-      <c r="I94" t="n">
-        <v>153.4940952380952</v>
-      </c>
-      <c r="J94" t="inlineStr"/>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>SO-1013166</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1</v>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Pack_44Filler</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Pack 44 Filler Material</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>508</v>
+      </c>
+      <c r="H93" t="n">
+        <v>203.2</v>
+      </c>
+      <c r="I93" t="n">
+        <v>268.6868390022676</v>
+      </c>
+      <c r="J93" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -13187,23 +13198,23 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2SS.145.15LNW</t>
+          <t>6VR.145.15LNW</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E95" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G95" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H95" t="n">
         <v>177.8</v>
       </c>
       <c r="I95" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J95" t="inlineStr"/>
     </row>
@@ -13218,7 +13229,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>1TJT.145.15LNW</t>
+          <t>2SS.145.15LNW</t>
         </is>
       </c>
       <c r="D96" t="n">
@@ -13228,13 +13239,13 @@
         <v>20</v>
       </c>
       <c r="G96" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H96" t="n">
         <v>177.8</v>
       </c>
       <c r="I96" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J96" t="inlineStr"/>
     </row>
@@ -13249,23 +13260,23 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>JT23.145.15LNW</t>
+          <t>1TJT.145.15LNW</t>
         </is>
       </c>
       <c r="D97" t="n">
         <v>1</v>
       </c>
       <c r="E97" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G97" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H97" t="n">
         <v>177.8</v>
       </c>
       <c r="I97" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J97" t="inlineStr"/>
     </row>
@@ -13280,23 +13291,23 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>JT23C.145.15LNW</t>
+          <t>JT23.145.15LNW</t>
         </is>
       </c>
       <c r="D98" t="n">
         <v>1</v>
       </c>
       <c r="E98" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G98" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H98" t="n">
         <v>177.8</v>
       </c>
       <c r="I98" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J98" t="inlineStr"/>
     </row>
@@ -13311,23 +13322,23 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>2TB.145.15LNW</t>
+          <t>JT23C.145.15LNW</t>
         </is>
       </c>
       <c r="D99" t="n">
         <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G99" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H99" t="n">
         <v>177.8</v>
       </c>
       <c r="I99" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J99" t="inlineStr"/>
     </row>
@@ -13342,23 +13353,23 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>2TB.145.15LNW</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E100" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G100" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H100" t="n">
         <v>177.8</v>
       </c>
       <c r="I100" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J100" t="inlineStr"/>
     </row>
@@ -13373,28 +13384,23 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E101" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G101" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H101" t="n">
         <v>177.8</v>
       </c>
       <c r="I101" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J101" t="inlineStr"/>
     </row>
@@ -13409,7 +13415,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -13420,17 +13426,17 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G102" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H102" t="n">
         <v>177.8</v>
       </c>
       <c r="I102" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J102" t="inlineStr"/>
     </row>
@@ -13445,7 +13451,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D103" t="n">
@@ -13456,17 +13462,17 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H103" t="n">
         <v>177.8</v>
       </c>
       <c r="I103" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J103" t="inlineStr"/>
     </row>
@@ -13481,7 +13487,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D104" t="n">
@@ -13492,17 +13498,17 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H104" t="n">
         <v>177.8</v>
       </c>
       <c r="I104" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J104" t="inlineStr"/>
     </row>
@@ -13517,7 +13523,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D105" t="n">
@@ -13528,17 +13534,17 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H105" t="n">
         <v>177.8</v>
       </c>
       <c r="I105" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J105" t="inlineStr"/>
     </row>
@@ -13553,28 +13559,28 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
         <v>1</v>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H106" t="n">
         <v>177.8</v>
       </c>
       <c r="I106" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J106" t="inlineStr"/>
     </row>
@@ -13589,61 +13595,66 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Pack_44Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E107" t="n">
         <v>1</v>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Pack 44 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>406.4</v>
+        <v>381</v>
       </c>
       <c r="H107" t="n">
         <v>177.8</v>
       </c>
       <c r="I107" t="n">
-        <v>153.4940952380952</v>
+        <v>152.224253968254</v>
       </c>
       <c r="J107" t="inlineStr"/>
     </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>SO-1013111</t>
-        </is>
-      </c>
-      <c r="B109" t="n">
-        <v>1</v>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>6VR.289.15DWO</t>
-        </is>
-      </c>
-      <c r="D109" t="n">
-        <v>5</v>
-      </c>
-      <c r="E109" t="n">
-        <v>8</v>
-      </c>
-      <c r="G109" t="n">
-        <v>584.2</v>
-      </c>
-      <c r="H109" t="n">
-        <v>228.6</v>
-      </c>
-      <c r="I109" t="n">
-        <v>482.2967664399093</v>
-      </c>
-      <c r="J109" t="inlineStr"/>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>SO-1013210</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>1</v>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Pack_44Filler</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Pack 44 Filler Material</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>381</v>
+      </c>
+      <c r="H108" t="n">
+        <v>177.8</v>
+      </c>
+      <c r="I108" t="n">
+        <v>152.224253968254</v>
+      </c>
+      <c r="J108" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -13656,11 +13667,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>6V.289.15ISL</t>
+          <t>6VR.289.15DWO</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E110" t="n">
         <v>8</v>
@@ -13687,14 +13698,14 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>JT23.145.15DWO</t>
+          <t>6V.289.15ISL</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G111" t="n">
         <v>584.2</v>
@@ -13718,7 +13729,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>JT23.145.15ISL</t>
+          <t>JT23.145.15DWO</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -13749,14 +13760,14 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>2COR1.145.15ISL</t>
+          <t>JT23.145.15ISL</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E113" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G113" t="n">
         <v>584.2</v>
@@ -13780,14 +13791,14 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>2BA.145.15OBL</t>
+          <t>2COR1.145.15ISL</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E114" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G114" t="n">
         <v>584.2</v>
@@ -13811,14 +13822,14 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>JT23C.145.15DWO</t>
+          <t>2BA.145.15OBL</t>
         </is>
       </c>
       <c r="D115" t="n">
         <v>1</v>
       </c>
       <c r="E115" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G115" t="n">
         <v>584.2</v>
@@ -13842,14 +13853,14 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>2TB.145.15DWO</t>
+          <t>JT23C.145.15DWO</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E116" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G116" t="n">
         <v>584.2</v>
@@ -13873,11 +13884,11 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>2FR.145.15DWO</t>
+          <t>2TB.145.15DWO</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E117" t="n">
         <v>10</v>
@@ -13904,14 +13915,14 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>2COR2.145.15ISL</t>
+          <t>2FR.145.15DWO</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G118" t="n">
         <v>584.2</v>
@@ -13935,14 +13946,14 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>2COR2.145.15ISL</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E119" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G119" t="n">
         <v>584.2</v>
@@ -13966,19 +13977,14 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E120" t="n">
-        <v>1</v>
-      </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G120" t="n">
         <v>584.2</v>
@@ -14002,7 +14008,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D121" t="n">
@@ -14013,7 +14019,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G121" t="n">
@@ -14038,7 +14044,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D122" t="n">
@@ -14049,7 +14055,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -14074,7 +14080,7 @@
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D123" t="n">
@@ -14085,7 +14091,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -14110,7 +14116,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D124" t="n">
@@ -14121,7 +14127,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -14146,18 +14152,18 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" t="n">
         <v>1</v>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -14182,18 +14188,18 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Pack_62Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E126" t="n">
         <v>1</v>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Pack 62 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G126" t="n">
@@ -14207,36 +14213,41 @@
       </c>
       <c r="J126" t="inlineStr"/>
     </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>SO-1013148</t>
-        </is>
-      </c>
-      <c r="B128" t="n">
-        <v>1</v>
-      </c>
-      <c r="C128" t="inlineStr">
-        <is>
-          <t>6VR.289.15LBB</t>
-        </is>
-      </c>
-      <c r="D128" t="n">
-        <v>35</v>
-      </c>
-      <c r="E128" t="n">
-        <v>8</v>
-      </c>
-      <c r="G128" t="n">
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>SO-1013111</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Pack_62Filler</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" t="n">
+        <v>1</v>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Pack 62 Filler Material</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
         <v>584.2</v>
       </c>
-      <c r="H128" t="n">
-        <v>584.1999999999999</v>
-      </c>
-      <c r="I128" t="n">
-        <v>1833.95166893424</v>
-      </c>
-      <c r="J128" t="inlineStr"/>
+      <c r="H127" t="n">
+        <v>228.6</v>
+      </c>
+      <c r="I127" t="n">
+        <v>482.2967664399093</v>
+      </c>
+      <c r="J127" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -14249,14 +14260,14 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>2BTBSS.145.15OBL</t>
+          <t>6VR.289.15LBB</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E129" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G129" t="n">
         <v>584.2</v>
@@ -14280,11 +14291,11 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>TGBJKIT</t>
+          <t>2BTBSS.145.15OBL</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E130" t="n">
         <v>10</v>
@@ -14311,14 +14322,14 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>TGBJKIT</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E131" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="G131" t="n">
         <v>584.2</v>
@@ -14342,19 +14353,14 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E132" t="n">
-        <v>1</v>
-      </c>
-      <c r="F132" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G132" t="n">
         <v>584.2</v>
@@ -14378,7 +14384,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D133" t="n">
@@ -14389,7 +14395,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -14414,7 +14420,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D134" t="n">
@@ -14425,7 +14431,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G134" t="n">
@@ -14450,7 +14456,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D135" t="n">
@@ -14461,7 +14467,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G135" t="n">
@@ -14486,7 +14492,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D136" t="n">
@@ -14497,7 +14503,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G136" t="n">
@@ -14522,18 +14528,18 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E137" t="n">
         <v>1</v>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G137" t="n">
@@ -14554,27 +14560,32 @@
         </is>
       </c>
       <c r="B138" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Pack_Pad_19_3680</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
         <v>2</v>
       </c>
-      <c r="C138" t="inlineStr">
-        <is>
-          <t>6VR.289.15LBB</t>
-        </is>
-      </c>
-      <c r="D138" t="n">
-        <v>10</v>
-      </c>
       <c r="E138" t="n">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+        </is>
       </c>
       <c r="G138" t="n">
         <v>584.2</v>
       </c>
       <c r="H138" t="n">
-        <v>520.7</v>
+        <v>584.1999999999999</v>
       </c>
       <c r="I138" t="n">
-        <v>960.5608072562358</v>
+        <v>1833.95166893424</v>
       </c>
       <c r="J138" t="inlineStr"/>
     </row>
@@ -14589,11 +14600,11 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>3V.145.15LBB</t>
+          <t>6VR.289.15LBB</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E139" t="n">
         <v>8</v>
@@ -14620,14 +14631,14 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>JT23.145.15LBB</t>
+          <t>3V.145.15LBB</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E140" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G140" t="n">
         <v>584.2</v>
@@ -14651,11 +14662,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>2BA.145.15OBL</t>
+          <t>JT23.145.15LBB</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E141" t="n">
         <v>10</v>
@@ -14682,14 +14693,14 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>JT23C.145.15LBB</t>
+          <t>2BA.145.15OBL</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E142" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G142" t="n">
         <v>584.2</v>
@@ -14713,14 +14724,14 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>2TB.145.15LBB</t>
+          <t>JT23C.145.15LBB</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E143" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G143" t="n">
         <v>584.2</v>
@@ -14744,14 +14755,14 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>CLIP.N1500</t>
+          <t>2TB.145.15LBB</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E144" t="n">
-        <v>1500</v>
+        <v>10</v>
       </c>
       <c r="G144" t="n">
         <v>584.2</v>
@@ -14775,14 +14786,14 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>2FR.145.15LBB</t>
+          <t>CLIP.N1500</t>
         </is>
       </c>
       <c r="D145" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E145" t="n">
-        <v>10</v>
+        <v>1500</v>
       </c>
       <c r="G145" t="n">
         <v>584.2</v>
@@ -14806,19 +14817,14 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>2FR.145.15LBB</t>
         </is>
       </c>
       <c r="D146" t="n">
         <v>1</v>
       </c>
       <c r="E146" t="n">
-        <v>1</v>
-      </c>
-      <c r="F146" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>10</v>
       </c>
       <c r="G146" t="n">
         <v>584.2</v>
@@ -14842,7 +14848,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D147" t="n">
@@ -14853,7 +14859,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G147" t="n">
@@ -14878,7 +14884,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D148" t="n">
@@ -14889,7 +14895,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G148" t="n">
@@ -14914,7 +14920,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D149" t="n">
@@ -14925,7 +14931,7 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G149" t="n">
@@ -14950,7 +14956,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D150" t="n">
@@ -14961,7 +14967,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G150" t="n">
@@ -14986,18 +14992,18 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D151" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E151" t="n">
         <v>1</v>
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G151" t="n">
@@ -15022,18 +15028,18 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Pack_44Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D152" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E152" t="n">
         <v>1</v>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>Pack 44 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G152" t="n">
@@ -15047,36 +15053,41 @@
       </c>
       <c r="J152" t="inlineStr"/>
     </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>SO-1013122</t>
-        </is>
-      </c>
-      <c r="B154" t="n">
-        <v>1</v>
-      </c>
-      <c r="C154" t="inlineStr">
-        <is>
-          <t>6VR.289.15IRW</t>
-        </is>
-      </c>
-      <c r="D154" t="n">
-        <v>7</v>
-      </c>
-      <c r="E154" t="n">
-        <v>8</v>
-      </c>
-      <c r="G154" t="n">
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>SO-1013148</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>2</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>Pack_44Filler</t>
+        </is>
+      </c>
+      <c r="D153" t="n">
+        <v>3</v>
+      </c>
+      <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Pack 44 Filler Material</t>
+        </is>
+      </c>
+      <c r="G153" t="n">
         <v>584.2</v>
       </c>
-      <c r="H154" t="n">
-        <v>228.6</v>
-      </c>
-      <c r="I154" t="n">
-        <v>498.6188117913832</v>
-      </c>
-      <c r="J154" t="inlineStr"/>
+      <c r="H153" t="n">
+        <v>520.7</v>
+      </c>
+      <c r="I153" t="n">
+        <v>960.5608072562358</v>
+      </c>
+      <c r="J153" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -15089,11 +15100,11 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>6VR.145.15IRW</t>
+          <t>6VR.289.15IRW</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E155" t="n">
         <v>8</v>
@@ -15120,14 +15131,14 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>2SS.145.15ISL</t>
+          <t>6VR.145.15IRW</t>
         </is>
       </c>
       <c r="D156" t="n">
         <v>1</v>
       </c>
       <c r="E156" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G156" t="n">
         <v>584.2</v>
@@ -15151,14 +15162,14 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>JT23.145.15IRW</t>
+          <t>2SS.145.15ISL</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G157" t="n">
         <v>584.2</v>
@@ -15182,11 +15193,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>JT23.145.15ISL</t>
+          <t>JT23.145.15IRW</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E158" t="n">
         <v>10</v>
@@ -15213,14 +15224,14 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>2COR1.145.15IRW</t>
+          <t>JT23.145.15ISL</t>
         </is>
       </c>
       <c r="D159" t="n">
         <v>1</v>
       </c>
       <c r="E159" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G159" t="n">
         <v>584.2</v>
@@ -15244,14 +15255,14 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>2FR.145.15ISL</t>
+          <t>2COR1.145.15IRW</t>
         </is>
       </c>
       <c r="D160" t="n">
         <v>1</v>
       </c>
       <c r="E160" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G160" t="n">
         <v>584.2</v>
@@ -15275,14 +15286,14 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>2COR2.145.15IRW</t>
+          <t>2FR.145.15ISL</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G161" t="n">
         <v>584.2</v>
@@ -15306,14 +15317,14 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>2COR2.145.15IRW</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E162" t="n">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="G162" t="n">
         <v>584.2</v>
@@ -15337,19 +15348,14 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E163" t="n">
-        <v>1</v>
-      </c>
-      <c r="F163" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G163" t="n">
         <v>584.2</v>
@@ -15373,7 +15379,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -15384,7 +15390,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G164" t="n">
@@ -15409,7 +15415,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D165" t="n">
@@ -15420,7 +15426,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G165" t="n">
@@ -15445,7 +15451,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D166" t="n">
@@ -15456,7 +15462,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G166" t="n">
@@ -15481,7 +15487,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D167" t="n">
@@ -15492,7 +15498,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G167" t="n">
@@ -15517,18 +15523,18 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E168" t="n">
         <v>1</v>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G168" t="n">
@@ -15553,18 +15559,18 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Pack_44Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E169" t="n">
         <v>1</v>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>Pack 44 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G169" t="n">
@@ -15578,36 +15584,41 @@
       </c>
       <c r="J169" t="inlineStr"/>
     </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>SO-1013129</t>
-        </is>
-      </c>
-      <c r="B171" t="n">
-        <v>1</v>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>6VR.145.15WCD</t>
-        </is>
-      </c>
-      <c r="D171" t="n">
-        <v>5</v>
-      </c>
-      <c r="E171" t="n">
-        <v>8</v>
-      </c>
-      <c r="G171" t="n">
-        <v>406.3999999999999</v>
-      </c>
-      <c r="H171" t="n">
-        <v>177.8</v>
-      </c>
-      <c r="I171" t="n">
-        <v>168.5552698412698</v>
-      </c>
-      <c r="J171" t="inlineStr"/>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>SO-1013122</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>1</v>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>Pack_44Filler</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" t="n">
+        <v>1</v>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Pack 44 Filler Material</t>
+        </is>
+      </c>
+      <c r="G170" t="n">
+        <v>584.2</v>
+      </c>
+      <c r="H170" t="n">
+        <v>228.6</v>
+      </c>
+      <c r="I170" t="n">
+        <v>498.6188117913832</v>
+      </c>
+      <c r="J170" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -15620,23 +15631,23 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>CLIP.N100</t>
+          <t>6VR.145.15WCD</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="E172" t="n">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="G172" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H172" t="n">
         <v>177.8</v>
       </c>
       <c r="I172" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J172" t="inlineStr"/>
     </row>
@@ -15651,28 +15662,23 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Pack_Angle</t>
+          <t>CLIP.N100</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E173" t="n">
-        <v>1</v>
-      </c>
-      <c r="F173" t="inlineStr">
-        <is>
-          <t>PRINTED ANGLEBOARD 3680mm</t>
-        </is>
+        <v>100</v>
       </c>
       <c r="G173" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H173" t="n">
         <v>177.8</v>
       </c>
       <c r="I173" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J173" t="inlineStr"/>
     </row>
@@ -15687,7 +15693,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Pack_1x4x19_Dun</t>
+          <t>Pack_Angle</t>
         </is>
       </c>
       <c r="D174" t="n">
@@ -15698,17 +15704,17 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
+          <t>PRINTED ANGLEBOARD 3680mm</t>
         </is>
       </c>
       <c r="G174" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H174" t="n">
         <v>177.8</v>
       </c>
       <c r="I174" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J174" t="inlineStr"/>
     </row>
@@ -15723,7 +15729,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Pack_2x3x19_Dun</t>
+          <t>Pack_1x4x19_Dun</t>
         </is>
       </c>
       <c r="D175" t="n">
@@ -15734,17 +15740,17 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
+          <t>1" X 4" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G175" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H175" t="n">
         <v>177.8</v>
       </c>
       <c r="I175" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J175" t="inlineStr"/>
     </row>
@@ -15759,7 +15765,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Pack_Sub_Bundl_Wrp_3680</t>
+          <t>Pack_2x3x19_Dun</t>
         </is>
       </c>
       <c r="D176" t="n">
@@ -15770,17 +15776,17 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
+          <t>2" X 3" X 19" DUNNAGE 3680mm</t>
         </is>
       </c>
       <c r="G176" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H176" t="n">
         <v>177.8</v>
       </c>
       <c r="I176" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J176" t="inlineStr"/>
     </row>
@@ -15795,7 +15801,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Pack_Mst_Bundl_Wrp_3680</t>
+          <t>Pack_Sub_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D177" t="n">
@@ -15806,17 +15812,17 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>Master Bundle - Stretch Wrap 3680mm</t>
+          <t>Sub-Bundle Wrap - Crepe Paper/Stretch Film 3680mm</t>
         </is>
       </c>
       <c r="G177" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H177" t="n">
         <v>177.8</v>
       </c>
       <c r="I177" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J177" t="inlineStr"/>
     </row>
@@ -15831,28 +15837,28 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Pack_Pad_19_3680</t>
+          <t>Pack_Mst_Bundl_Wrp_3680</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E178" t="n">
         <v>1</v>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
+          <t>Master Bundle - Stretch Wrap 3680mm</t>
         </is>
       </c>
       <c r="G178" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H178" t="n">
         <v>177.8</v>
       </c>
       <c r="I178" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J178" t="inlineStr"/>
     </row>
@@ -15867,28 +15873,28 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Pack_62Filler</t>
+          <t>Pack_Pad_19_3680</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E179" t="n">
         <v>1</v>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>Pack 62 Filler Material</t>
+          <t>PAD - 19" X 144" DW ECT #3 WHITE 3680mm</t>
         </is>
       </c>
       <c r="G179" t="n">
-        <v>406.3999999999999</v>
+        <v>279.4</v>
       </c>
       <c r="H179" t="n">
         <v>177.8</v>
       </c>
       <c r="I179" t="n">
-        <v>168.5552698412698</v>
+        <v>147.2396507936508</v>
       </c>
       <c r="J179" t="inlineStr"/>
     </row>
@@ -15913,13 +15919,13 @@
         <v>8</v>
       </c>
       <c r="G181" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H181" t="n">
         <v>177.8</v>
       </c>
       <c r="I181" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J181" t="inlineStr"/>
     </row>
@@ -15938,19 +15944,19 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E182" t="n">
         <v>100</v>
       </c>
       <c r="G182" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H182" t="n">
         <v>177.8</v>
       </c>
       <c r="I182" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J182" t="inlineStr"/>
     </row>
@@ -15980,13 +15986,13 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H183" t="n">
         <v>177.8</v>
       </c>
       <c r="I183" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J183" t="inlineStr"/>
     </row>
@@ -16016,13 +16022,13 @@
         </is>
       </c>
       <c r="G184" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H184" t="n">
         <v>177.8</v>
       </c>
       <c r="I184" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J184" t="inlineStr"/>
     </row>
@@ -16052,13 +16058,13 @@
         </is>
       </c>
       <c r="G185" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H185" t="n">
         <v>177.8</v>
       </c>
       <c r="I185" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J185" t="inlineStr"/>
     </row>
@@ -16088,13 +16094,13 @@
         </is>
       </c>
       <c r="G186" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H186" t="n">
         <v>177.8</v>
       </c>
       <c r="I186" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J186" t="inlineStr"/>
     </row>
@@ -16124,13 +16130,13 @@
         </is>
       </c>
       <c r="G187" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H187" t="n">
         <v>177.8</v>
       </c>
       <c r="I187" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J187" t="inlineStr"/>
     </row>
@@ -16160,13 +16166,13 @@
         </is>
       </c>
       <c r="G188" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H188" t="n">
         <v>177.8</v>
       </c>
       <c r="I188" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J188" t="inlineStr"/>
     </row>
@@ -16191,13 +16197,13 @@
         <v>8</v>
       </c>
       <c r="G190" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H190" t="n">
         <v>177.8</v>
       </c>
       <c r="I190" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J190" t="inlineStr"/>
     </row>
@@ -16216,19 +16222,19 @@
         </is>
       </c>
       <c r="D191" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E191" t="n">
         <v>100</v>
       </c>
       <c r="G191" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H191" t="n">
         <v>177.8</v>
       </c>
       <c r="I191" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J191" t="inlineStr"/>
     </row>
@@ -16258,13 +16264,13 @@
         </is>
       </c>
       <c r="G192" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H192" t="n">
         <v>177.8</v>
       </c>
       <c r="I192" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J192" t="inlineStr"/>
     </row>
@@ -16294,13 +16300,13 @@
         </is>
       </c>
       <c r="G193" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H193" t="n">
         <v>177.8</v>
       </c>
       <c r="I193" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J193" t="inlineStr"/>
     </row>
@@ -16330,13 +16336,13 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H194" t="n">
         <v>177.8</v>
       </c>
       <c r="I194" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J194" t="inlineStr"/>
     </row>
@@ -16366,13 +16372,13 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H195" t="n">
         <v>177.8</v>
       </c>
       <c r="I195" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J195" t="inlineStr"/>
     </row>
@@ -16402,13 +16408,13 @@
         </is>
       </c>
       <c r="G196" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H196" t="n">
         <v>177.8</v>
       </c>
       <c r="I196" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J196" t="inlineStr"/>
     </row>
@@ -16438,13 +16444,13 @@
         </is>
       </c>
       <c r="G197" t="n">
-        <v>228.6</v>
+        <v>177.8</v>
       </c>
       <c r="H197" t="n">
         <v>177.8</v>
       </c>
       <c r="I197" t="n">
-        <v>174.5412380952381</v>
+        <v>170.7317142857143</v>
       </c>
       <c r="J197" t="inlineStr"/>
     </row>

</xml_diff>